<commit_message>
will not include ~.xlxs in displaying excel files
</commit_message>
<xml_diff>
--- a/terminal/sample_exam_files/test.xlsx
+++ b/terminal/sample_exam_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\razstvien\projects\QuizSheetLoader\terminal\sample_exam_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4405253-5518-4AD2-962F-3741173C1255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D789FA-9C58-4A4A-96AD-821777E321D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions@multiplechoice" sheetId="3" r:id="rId1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23C0BC9-1719-4D08-8F30-76385AB08B22}">
   <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +838,7 @@
       <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -854,9 +854,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
+      <c r="C3" s="13"/>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
@@ -870,9 +868,7 @@
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
+      <c r="C4" s="13"/>
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
@@ -886,9 +882,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
+      <c r="C5" s="13"/>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2508,7 +2502,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="119">
+    <mergeCell ref="C2:C5"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B34:B37"/>
@@ -2943,7 +2938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EA16EF-B104-4EA3-AE5D-62121FAFDAC9}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix re randomize after choosing wrong answer in multiple choice category
</commit_message>
<xml_diff>
--- a/terminal/sample_exam_files/test.xlsx
+++ b/terminal/sample_exam_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\razstvien\projects\QuizSheetLoader\terminal\sample_exam_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AECD11-6E34-4415-BDE5-0F7DA372323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D96FA1-A067-4D57-8303-2D74F9739A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions@multiplechoice" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Questions</t>
   </si>
@@ -63,6 +63,39 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>A travel company is in the early stages of developing a new application and wants to test it on a variety of configurations: different operating systems, processors, and storage options. What cloud computing option should they use?</t>
+  </si>
+  <si>
+    <t>Colocation</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>Virtual machine instances</t>
+  </si>
+  <si>
+    <t>A local development environment</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>They allow for extensive testing across different configurations of OS, processors, and storage.</t>
+  </si>
+  <si>
+    <t>This option involves physical servers in a data center and lacks the flexibility needed for rapid testing across diverse configurations.</t>
+  </si>
+  <si>
+    <t>This flexibility is ideal for testing and development purposes, as it enables the company to simulate various environments and configurations without the need for physical hardware.</t>
+  </si>
+  <si>
+    <t>This limits testing to a single setup and doesn’t provide the variety needed for thorough application testing.</t>
   </si>
 </sst>
 </file>
@@ -136,16 +169,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -165,18 +195,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -186,23 +204,35 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -221,6 +251,18 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -235,14 +277,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29CFBDFD-64DF-4029-945F-27C6A43EF17A}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29CFBDFD-64DF-4029-945F-27C6A43EF17A}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E6" xr:uid="{29CFBDFD-64DF-4029-945F-27C6A43EF17A}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{B18A27A8-3AFE-428E-AD75-ED0B50BA1894}" name="Index" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{072BA199-D5A2-4ACD-86F1-4D86A88AAD41}" name="Questions" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C6F80DE2-4F15-4CC1-B64A-B90C37158F78}" name="Answer" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6B5EDEA6-9A27-4DF7-96DE-DE4771766797}" name="Points" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{26DA488D-68EB-4998-ACA5-825E864F5120}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B18A27A8-3AFE-428E-AD75-ED0B50BA1894}" name="Index" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{072BA199-D5A2-4ACD-86F1-4D86A88AAD41}" name="Questions" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C6F80DE2-4F15-4CC1-B64A-B90C37158F78}" name="Answer" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6B5EDEA6-9A27-4DF7-96DE-DE4771766797}" name="Points" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{26DA488D-68EB-4998-ACA5-825E864F5120}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -568,7 +610,7 @@
   <dimension ref="A1:F237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,1534 +625,1475 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="D6" s="7"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="D7" s="8"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="D8" s="7"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="D9" s="9"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="D10" s="7"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="D11" s="7"/>
-      <c r="F11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="D12" s="7"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
-      <c r="D13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="D17" s="8"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="D18" s="7"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="D19" s="7"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="D20" s="6"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="D21" s="7"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="D22" s="7"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
-      <c r="D23" s="8"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="D24" s="7"/>
-      <c r="F24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="D25" s="9"/>
-      <c r="F25" s="5"/>
+      <c r="D25" s="8"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
-      <c r="D26" s="7"/>
-      <c r="F26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
-      <c r="D27" s="7"/>
-      <c r="F27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="D28" s="7"/>
-      <c r="F28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
-      <c r="D29" s="6"/>
-      <c r="F29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
-      <c r="D30" s="7"/>
-      <c r="F30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
-      <c r="D31" s="7"/>
-      <c r="F31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
-      <c r="D32" s="6"/>
-      <c r="F32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
-      <c r="D33" s="6"/>
-      <c r="F33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
-      <c r="D34" s="7"/>
-      <c r="F34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
-      <c r="D35" s="8"/>
-      <c r="F35" s="5"/>
+      <c r="D35" s="7"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
-      <c r="D36" s="7"/>
-      <c r="F36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
-      <c r="D37" s="9"/>
-      <c r="F37" s="5"/>
+      <c r="D37" s="8"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
-      <c r="B38" s="11"/>
-      <c r="D38" s="7"/>
-      <c r="F38" s="5"/>
+      <c r="B38" s="14"/>
+      <c r="D38" s="6"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
-      <c r="D39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="B39" s="14"/>
+      <c r="D39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
-      <c r="B40" s="11"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="B40" s="14"/>
+      <c r="D40" s="4"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
-      <c r="B41" s="11"/>
-      <c r="D41" s="6"/>
-      <c r="F41" s="5"/>
+      <c r="B41" s="14"/>
+      <c r="D41" s="5"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
-      <c r="D42" s="7"/>
-      <c r="F42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
-      <c r="D43" s="6"/>
-      <c r="F43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
-      <c r="D44" s="7"/>
-      <c r="F44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
-      <c r="D45" s="7"/>
-      <c r="F45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
-      <c r="D46" s="7"/>
-      <c r="F46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
-      <c r="D47" s="7"/>
-      <c r="F47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
-      <c r="D48" s="6"/>
-      <c r="F48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
-      <c r="D49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="D49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
-      <c r="D50" s="7"/>
-      <c r="F50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
-      <c r="D51" s="7"/>
-      <c r="F51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
-      <c r="D52" s="7"/>
-      <c r="F52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
-      <c r="F53" s="5"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
-      <c r="D54" s="7"/>
-      <c r="F54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
-      <c r="D55" s="7"/>
-      <c r="F55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
-      <c r="D56" s="8"/>
-      <c r="F56" s="5"/>
+      <c r="D56" s="7"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
-      <c r="F57" s="5"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="12"/>
-      <c r="D58" s="7"/>
-      <c r="F58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="12"/>
-      <c r="D59" s="7"/>
-      <c r="F59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="12"/>
-      <c r="D60" s="7"/>
-      <c r="F60" s="5"/>
+      <c r="D60" s="6"/>
+      <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="12"/>
-      <c r="F61" s="5"/>
+      <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="12"/>
-      <c r="D62" s="7"/>
-      <c r="F62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="12"/>
-      <c r="D63" s="7"/>
-      <c r="F63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="12"/>
-      <c r="D64" s="8"/>
-      <c r="F64" s="5"/>
+      <c r="D64" s="7"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="12"/>
-      <c r="F65" s="5"/>
+      <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
-      <c r="D66" s="7"/>
-      <c r="F66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="12"/>
-      <c r="D67" s="7"/>
-      <c r="F67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="F67" s="4"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="12"/>
-      <c r="D68" s="7"/>
-      <c r="F68" s="5"/>
+      <c r="D68" s="6"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="12"/>
-      <c r="D69" s="8"/>
-      <c r="F69" s="5"/>
+      <c r="D69" s="7"/>
+      <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="12"/>
-      <c r="D70" s="7"/>
-      <c r="F70" s="5"/>
+      <c r="D70" s="6"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="12"/>
-      <c r="D71" s="7"/>
-      <c r="F71" s="5"/>
+      <c r="D71" s="6"/>
+      <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="12"/>
-      <c r="D72" s="7"/>
-      <c r="F72" s="5"/>
+      <c r="D72" s="6"/>
+      <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="12"/>
       <c r="B73" s="12"/>
-      <c r="D73" s="6"/>
-      <c r="F73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="12"/>
-      <c r="D74" s="7"/>
-      <c r="F74" s="5"/>
+      <c r="D74" s="6"/>
+      <c r="F74" s="4"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="12"/>
       <c r="B75" s="12"/>
-      <c r="D75" s="7"/>
-      <c r="F75" s="5"/>
+      <c r="D75" s="6"/>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="12"/>
       <c r="B76" s="12"/>
-      <c r="D76" s="8"/>
-      <c r="F76" s="5"/>
+      <c r="D76" s="7"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="12"/>
       <c r="B77" s="12"/>
-      <c r="D77" s="9"/>
-      <c r="F77" s="5"/>
+      <c r="D77" s="8"/>
+      <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12"/>
       <c r="B78" s="12"/>
-      <c r="D78" s="8"/>
-      <c r="F78" s="5"/>
+      <c r="D78" s="7"/>
+      <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
       <c r="B79" s="12"/>
-      <c r="D79" s="7"/>
-      <c r="F79" s="5"/>
+      <c r="D79" s="6"/>
+      <c r="F79" s="4"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>
       <c r="B80" s="12"/>
-      <c r="D80" s="7"/>
-      <c r="F80" s="5"/>
+      <c r="D80" s="6"/>
+      <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="12"/>
-      <c r="D81" s="9"/>
-      <c r="F81" s="5"/>
+      <c r="D81" s="8"/>
+      <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
       <c r="B82" s="12"/>
-      <c r="D82" s="7"/>
-      <c r="F82" s="5"/>
+      <c r="D82" s="6"/>
+      <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="12"/>
       <c r="B83" s="12"/>
-      <c r="D83" s="7"/>
-      <c r="F83" s="5"/>
+      <c r="D83" s="6"/>
+      <c r="F83" s="4"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
-      <c r="D84" s="7"/>
-      <c r="F84" s="5"/>
+      <c r="D84" s="6"/>
+      <c r="F84" s="4"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="12"/>
-      <c r="D85" s="8"/>
-      <c r="F85" s="5"/>
+      <c r="D85" s="7"/>
+      <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="12"/>
-      <c r="D86" s="8"/>
-      <c r="F86" s="5"/>
+      <c r="D86" s="7"/>
+      <c r="F86" s="4"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="12"/>
-      <c r="D87" s="7"/>
-      <c r="F87" s="5"/>
+      <c r="D87" s="6"/>
+      <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="12"/>
-      <c r="D88" s="7"/>
-      <c r="F88" s="5"/>
+      <c r="D88" s="6"/>
+      <c r="F88" s="4"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
       <c r="B89" s="12"/>
-      <c r="D89" s="7"/>
-      <c r="F89" s="5"/>
+      <c r="D89" s="6"/>
+      <c r="F89" s="4"/>
     </row>
     <row r="90" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
       <c r="B90" s="12"/>
-      <c r="D90" s="7"/>
-      <c r="F90" s="5"/>
+      <c r="D90" s="6"/>
+      <c r="F90" s="4"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="12"/>
-      <c r="D91" s="7"/>
-      <c r="F91" s="5"/>
+      <c r="D91" s="6"/>
+      <c r="F91" s="4"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="12"/>
-      <c r="D92" s="8"/>
-      <c r="F92" s="5"/>
+      <c r="D92" s="7"/>
+      <c r="F92" s="4"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="12"/>
-      <c r="D93" s="7"/>
-      <c r="F93" s="5"/>
+      <c r="D93" s="6"/>
+      <c r="F93" s="4"/>
     </row>
     <row r="94" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="12"/>
-      <c r="D94" s="7"/>
-      <c r="F94" s="5"/>
+      <c r="D94" s="6"/>
+      <c r="F94" s="4"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="12"/>
-      <c r="D95" s="7"/>
-      <c r="F95" s="5"/>
+      <c r="D95" s="6"/>
+      <c r="F95" s="4"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
       <c r="B96" s="12"/>
-      <c r="D96" s="8"/>
-      <c r="F96" s="5"/>
+      <c r="D96" s="7"/>
+      <c r="F96" s="4"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
       <c r="B97" s="12"/>
-      <c r="D97" s="9"/>
-      <c r="F97" s="5"/>
+      <c r="D97" s="8"/>
+      <c r="F97" s="4"/>
     </row>
     <row r="98" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="12"/>
-      <c r="D98" s="8"/>
-      <c r="F98" s="5"/>
+      <c r="D98" s="7"/>
+      <c r="F98" s="4"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="12"/>
-      <c r="D99" s="7"/>
-      <c r="F99" s="5"/>
+      <c r="D99" s="6"/>
+      <c r="F99" s="4"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
       <c r="B100" s="12"/>
-      <c r="D100" s="7"/>
-      <c r="F100" s="5"/>
+      <c r="D100" s="6"/>
+      <c r="F100" s="4"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="12"/>
-      <c r="D101" s="9"/>
-      <c r="F101" s="5"/>
+      <c r="D101" s="8"/>
+      <c r="F101" s="4"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="B102" s="12"/>
-      <c r="D102" s="8"/>
-      <c r="F102" s="5"/>
+      <c r="D102" s="7"/>
+      <c r="F102" s="4"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
-      <c r="D103" s="7"/>
-      <c r="F103" s="5"/>
+      <c r="D103" s="6"/>
+      <c r="F103" s="4"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
-      <c r="D104" s="7"/>
-      <c r="F104" s="5"/>
+      <c r="D104" s="6"/>
+      <c r="F104" s="4"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="12"/>
-      <c r="D105" s="9"/>
-      <c r="F105" s="5"/>
+      <c r="D105" s="8"/>
+      <c r="F105" s="4"/>
     </row>
     <row r="106" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="12"/>
-      <c r="D106" s="7"/>
-      <c r="F106" s="5"/>
+      <c r="D106" s="6"/>
+      <c r="F106" s="4"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
       <c r="B107" s="12"/>
-      <c r="D107" s="7"/>
-      <c r="F107" s="5"/>
+      <c r="D107" s="6"/>
+      <c r="F107" s="4"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
       <c r="B108" s="12"/>
-      <c r="D108" s="8"/>
-      <c r="F108" s="5"/>
+      <c r="D108" s="7"/>
+      <c r="F108" s="4"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
       <c r="B109" s="12"/>
-      <c r="D109" s="9"/>
-      <c r="F109" s="5"/>
+      <c r="D109" s="8"/>
+      <c r="F109" s="4"/>
     </row>
     <row r="110" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
       <c r="B110" s="12"/>
-      <c r="D110" s="7"/>
-      <c r="F110" s="5"/>
+      <c r="D110" s="6"/>
+      <c r="F110" s="4"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
       <c r="B111" s="12"/>
-      <c r="D111" s="7"/>
-      <c r="F111" s="5"/>
+      <c r="D111" s="6"/>
+      <c r="F111" s="4"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
       <c r="B112" s="12"/>
-      <c r="D112" s="8"/>
-      <c r="F112" s="4"/>
+      <c r="D112" s="7"/>
+      <c r="F112" s="3"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
-      <c r="D113" s="9"/>
-      <c r="F113" s="5"/>
+      <c r="D113" s="8"/>
+      <c r="F113" s="4"/>
     </row>
     <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="12"/>
-      <c r="D114" s="8"/>
-      <c r="F114" s="4"/>
+      <c r="D114" s="7"/>
+      <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="12"/>
-      <c r="D115" s="7"/>
-      <c r="F115" s="5"/>
+      <c r="D115" s="6"/>
+      <c r="F115" s="4"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
       <c r="B116" s="12"/>
-      <c r="D116" s="7"/>
-      <c r="F116" s="5"/>
+      <c r="D116" s="6"/>
+      <c r="F116" s="4"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
       <c r="B117" s="12"/>
-      <c r="D117" s="9"/>
-      <c r="F117" s="5"/>
+      <c r="D117" s="8"/>
+      <c r="F117" s="4"/>
     </row>
     <row r="118" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12"/>
       <c r="B118" s="12"/>
-      <c r="D118" s="7"/>
-      <c r="F118" s="5"/>
+      <c r="D118" s="6"/>
+      <c r="F118" s="4"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="12"/>
       <c r="B119" s="12"/>
-      <c r="D119" s="7"/>
-      <c r="F119" s="5"/>
+      <c r="D119" s="6"/>
+      <c r="F119" s="4"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="12"/>
       <c r="B120" s="12"/>
-      <c r="D120" s="7"/>
-      <c r="F120" s="4"/>
+      <c r="D120" s="6"/>
+      <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="12"/>
       <c r="B121" s="12"/>
-      <c r="D121" s="8"/>
-      <c r="F121" s="5"/>
+      <c r="D121" s="7"/>
+      <c r="F121" s="4"/>
     </row>
     <row r="122" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
-      <c r="D122" s="8"/>
-      <c r="F122" s="4"/>
+      <c r="D122" s="7"/>
+      <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="12"/>
-      <c r="D123" s="7"/>
-      <c r="F123" s="5"/>
+      <c r="D123" s="6"/>
+      <c r="F123" s="4"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="12"/>
-      <c r="D124" s="7"/>
-      <c r="F124" s="5"/>
+      <c r="D124" s="6"/>
+      <c r="F124" s="4"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="12"/>
-      <c r="D125" s="9"/>
-      <c r="F125" s="5"/>
+      <c r="D125" s="8"/>
+      <c r="F125" s="4"/>
     </row>
     <row r="126" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="12"/>
-      <c r="D126" s="7"/>
-      <c r="F126" s="5"/>
+      <c r="D126" s="6"/>
+      <c r="F126" s="4"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="12"/>
       <c r="B127" s="12"/>
-      <c r="D127" s="7"/>
-      <c r="F127" s="5"/>
+      <c r="D127" s="6"/>
+      <c r="F127" s="4"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
       <c r="B128" s="12"/>
-      <c r="D128" s="7"/>
-      <c r="F128" s="5"/>
+      <c r="D128" s="6"/>
+      <c r="F128" s="4"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="12"/>
       <c r="B129" s="12"/>
-      <c r="D129" s="8"/>
-      <c r="F129" s="5"/>
+      <c r="D129" s="7"/>
+      <c r="F129" s="4"/>
     </row>
     <row r="130" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
-      <c r="D130" s="8"/>
-      <c r="F130" s="5"/>
+      <c r="D130" s="7"/>
+      <c r="F130" s="4"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="12"/>
       <c r="B131" s="12"/>
-      <c r="D131" s="7"/>
-      <c r="F131" s="5"/>
+      <c r="D131" s="6"/>
+      <c r="F131" s="4"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
       <c r="B132" s="12"/>
-      <c r="D132" s="7"/>
-      <c r="F132" s="5"/>
+      <c r="D132" s="6"/>
+      <c r="F132" s="4"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="12"/>
       <c r="B133" s="12"/>
-      <c r="D133" s="9"/>
-      <c r="F133" s="5"/>
+      <c r="D133" s="8"/>
+      <c r="F133" s="4"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="12"/>
-      <c r="D134" s="7"/>
-      <c r="F134" s="5"/>
+      <c r="D134" s="6"/>
+      <c r="F134" s="4"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="12"/>
       <c r="B135" s="12"/>
-      <c r="D135" s="7"/>
-      <c r="F135" s="5"/>
+      <c r="D135" s="6"/>
+      <c r="F135" s="4"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12"/>
       <c r="B136" s="12"/>
-      <c r="D136" s="7"/>
-      <c r="F136" s="5"/>
+      <c r="D136" s="6"/>
+      <c r="F136" s="4"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12"/>
       <c r="B137" s="12"/>
-      <c r="D137" s="8"/>
-      <c r="F137" s="5"/>
+      <c r="D137" s="7"/>
+      <c r="F137" s="4"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="B138" s="12"/>
-      <c r="D138" s="7"/>
-      <c r="F138" s="5"/>
+      <c r="D138" s="6"/>
+      <c r="F138" s="4"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="B139" s="12"/>
-      <c r="D139" s="7"/>
-      <c r="F139" s="5"/>
+      <c r="D139" s="6"/>
+      <c r="F139" s="4"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
       <c r="B140" s="12"/>
-      <c r="D140" s="8"/>
-      <c r="F140" s="5"/>
+      <c r="D140" s="7"/>
+      <c r="F140" s="4"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
-      <c r="D141" s="9"/>
-      <c r="F141" s="5"/>
+      <c r="D141" s="8"/>
+      <c r="F141" s="4"/>
     </row>
     <row r="142" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12"/>
       <c r="B142" s="12"/>
-      <c r="D142" s="7"/>
-      <c r="F142" s="5"/>
+      <c r="D142" s="6"/>
+      <c r="F142" s="4"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="12"/>
-      <c r="D143" s="7"/>
-      <c r="F143" s="5"/>
+      <c r="D143" s="6"/>
+      <c r="F143" s="4"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="12"/>
       <c r="B144" s="12"/>
-      <c r="D144" s="7"/>
-      <c r="F144" s="5"/>
+      <c r="D144" s="6"/>
+      <c r="F144" s="4"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="12"/>
       <c r="B145" s="12"/>
-      <c r="D145" s="8"/>
-      <c r="F145" s="5"/>
+      <c r="D145" s="7"/>
+      <c r="F145" s="4"/>
     </row>
     <row r="146" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12"/>
       <c r="B146" s="12"/>
-      <c r="D146" s="8"/>
-      <c r="F146" s="5"/>
+      <c r="D146" s="7"/>
+      <c r="F146" s="4"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="12"/>
       <c r="B147" s="12"/>
-      <c r="D147" s="7"/>
-      <c r="F147" s="5"/>
+      <c r="D147" s="6"/>
+      <c r="F147" s="4"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="12"/>
       <c r="B148" s="12"/>
-      <c r="D148" s="7"/>
-      <c r="F148" s="5"/>
+      <c r="D148" s="6"/>
+      <c r="F148" s="4"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="12"/>
       <c r="B149" s="12"/>
-      <c r="D149" s="7"/>
-      <c r="F149" s="4"/>
+      <c r="D149" s="6"/>
+      <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12"/>
       <c r="B150" s="12"/>
-      <c r="D150" s="7"/>
-      <c r="F150" s="5"/>
+      <c r="D150" s="6"/>
+      <c r="F150" s="4"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="12"/>
-      <c r="D151" s="7"/>
-      <c r="F151" s="5"/>
+      <c r="D151" s="6"/>
+      <c r="F151" s="4"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="12"/>
-      <c r="D152" s="7"/>
-      <c r="F152" s="5"/>
+      <c r="D152" s="6"/>
+      <c r="F152" s="4"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="12"/>
-      <c r="D153" s="8"/>
-      <c r="F153" s="5"/>
+      <c r="D153" s="7"/>
+      <c r="F153" s="4"/>
     </row>
     <row r="154" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12"/>
       <c r="B154" s="12"/>
-      <c r="D154" s="8"/>
-      <c r="F154" s="5"/>
+      <c r="D154" s="7"/>
+      <c r="F154" s="4"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="12"/>
       <c r="B155" s="12"/>
-      <c r="D155" s="7"/>
-      <c r="F155" s="5"/>
+      <c r="D155" s="6"/>
+      <c r="F155" s="4"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="12"/>
       <c r="B156" s="12"/>
-      <c r="D156" s="7"/>
-      <c r="F156" s="5"/>
+      <c r="D156" s="6"/>
+      <c r="F156" s="4"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="12"/>
       <c r="B157" s="12"/>
-      <c r="D157" s="9"/>
-      <c r="F157" s="5"/>
+      <c r="D157" s="8"/>
+      <c r="F157" s="4"/>
     </row>
     <row r="158" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12"/>
       <c r="B158" s="12"/>
-      <c r="D158" s="7"/>
-      <c r="F158" s="5"/>
+      <c r="D158" s="6"/>
+      <c r="F158" s="4"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="12"/>
       <c r="B159" s="12"/>
-      <c r="D159" s="7"/>
-      <c r="F159" s="5"/>
+      <c r="D159" s="6"/>
+      <c r="F159" s="4"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="12"/>
       <c r="B160" s="12"/>
-      <c r="D160" s="8"/>
-      <c r="F160" s="5"/>
+      <c r="D160" s="7"/>
+      <c r="F160" s="4"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="12"/>
       <c r="B161" s="12"/>
-      <c r="D161" s="9"/>
-      <c r="F161" s="5"/>
+      <c r="D161" s="8"/>
+      <c r="F161" s="4"/>
     </row>
     <row r="162" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="12"/>
-      <c r="D162" s="8"/>
-      <c r="F162" s="5"/>
+      <c r="D162" s="7"/>
+      <c r="F162" s="4"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="12"/>
       <c r="B163" s="12"/>
-      <c r="D163" s="7"/>
-      <c r="F163" s="5"/>
+      <c r="D163" s="6"/>
+      <c r="F163" s="4"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="12"/>
       <c r="B164" s="12"/>
-      <c r="D164" s="7"/>
-      <c r="F164" s="5"/>
+      <c r="D164" s="6"/>
+      <c r="F164" s="4"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="12"/>
-      <c r="D165" s="9"/>
-      <c r="F165" s="4"/>
+      <c r="D165" s="8"/>
+      <c r="F165" s="3"/>
     </row>
     <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="12"/>
-      <c r="D166" s="7"/>
-      <c r="F166" s="5"/>
+      <c r="D166" s="6"/>
+      <c r="F166" s="4"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
       <c r="B167" s="12"/>
-      <c r="D167" s="8"/>
-      <c r="F167" s="5"/>
+      <c r="D167" s="7"/>
+      <c r="F167" s="4"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="12"/>
       <c r="B168" s="12"/>
-      <c r="D168" s="7"/>
-      <c r="F168" s="5"/>
+      <c r="D168" s="6"/>
+      <c r="F168" s="4"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="12"/>
       <c r="B169" s="12"/>
-      <c r="D169" s="9"/>
-      <c r="F169" s="4"/>
+      <c r="D169" s="8"/>
+      <c r="F169" s="3"/>
     </row>
     <row r="170" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
-      <c r="D170" s="8"/>
-      <c r="F170" s="5"/>
+      <c r="D170" s="7"/>
+      <c r="F170" s="4"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="12"/>
       <c r="B171" s="12"/>
-      <c r="D171" s="7"/>
-      <c r="F171" s="5"/>
+      <c r="D171" s="6"/>
+      <c r="F171" s="4"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="12"/>
       <c r="B172" s="12"/>
-      <c r="D172" s="7"/>
-      <c r="F172" s="5"/>
+      <c r="D172" s="6"/>
+      <c r="F172" s="4"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="12"/>
       <c r="B173" s="12"/>
-      <c r="D173" s="9"/>
-      <c r="F173" s="5"/>
+      <c r="D173" s="8"/>
+      <c r="F173" s="4"/>
     </row>
     <row r="174" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12"/>
       <c r="B174" s="12"/>
-      <c r="D174" s="8"/>
-      <c r="F174" s="5"/>
+      <c r="D174" s="7"/>
+      <c r="F174" s="4"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="12"/>
-      <c r="D175" s="7"/>
-      <c r="F175" s="5"/>
+      <c r="D175" s="6"/>
+      <c r="F175" s="4"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="12"/>
       <c r="B176" s="12"/>
-      <c r="D176" s="7"/>
-      <c r="F176" s="5"/>
+      <c r="D176" s="6"/>
+      <c r="F176" s="4"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="12"/>
       <c r="B177" s="12"/>
-      <c r="D177" s="9"/>
-      <c r="F177" s="5"/>
+      <c r="D177" s="8"/>
+      <c r="F177" s="4"/>
     </row>
     <row r="178" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
       <c r="B178" s="12"/>
-      <c r="D178" s="7"/>
-      <c r="F178" s="5"/>
+      <c r="D178" s="6"/>
+      <c r="F178" s="4"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="12"/>
       <c r="B179" s="12"/>
-      <c r="D179" s="7"/>
-      <c r="F179" s="5"/>
+      <c r="D179" s="6"/>
+      <c r="F179" s="4"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="12"/>
       <c r="B180" s="12"/>
-      <c r="D180" s="8"/>
-      <c r="F180" s="5"/>
+      <c r="D180" s="7"/>
+      <c r="F180" s="4"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
       <c r="B181" s="12"/>
-      <c r="D181" s="9"/>
-      <c r="F181" s="5"/>
+      <c r="D181" s="8"/>
+      <c r="F181" s="4"/>
     </row>
     <row r="182" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12"/>
       <c r="B182" s="12"/>
-      <c r="D182" s="7"/>
-      <c r="F182" s="5"/>
+      <c r="D182" s="6"/>
+      <c r="F182" s="4"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="12"/>
       <c r="B183" s="12"/>
-      <c r="D183" s="8"/>
-      <c r="F183" s="5"/>
+      <c r="D183" s="7"/>
+      <c r="F183" s="4"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="12"/>
       <c r="B184" s="12"/>
-      <c r="D184" s="7"/>
-      <c r="F184" s="5"/>
+      <c r="D184" s="6"/>
+      <c r="F184" s="4"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="12"/>
       <c r="B185" s="12"/>
-      <c r="D185" s="9"/>
-      <c r="F185" s="5"/>
+      <c r="D185" s="8"/>
+      <c r="F185" s="4"/>
     </row>
     <row r="186" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12"/>
       <c r="B186" s="12"/>
-      <c r="D186" s="7"/>
-      <c r="F186" s="5"/>
+      <c r="D186" s="6"/>
+      <c r="F186" s="4"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
       <c r="B187" s="12"/>
-      <c r="D187" s="8"/>
-      <c r="F187" s="5"/>
+      <c r="D187" s="7"/>
+      <c r="F187" s="4"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="12"/>
       <c r="B188" s="12"/>
-      <c r="D188" s="7"/>
-      <c r="F188" s="5"/>
+      <c r="D188" s="6"/>
+      <c r="F188" s="4"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="12"/>
       <c r="B189" s="12"/>
-      <c r="D189" s="9"/>
-      <c r="F189" s="5"/>
+      <c r="D189" s="8"/>
+      <c r="F189" s="4"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="12"/>
       <c r="B190" s="12"/>
-      <c r="D190" s="7"/>
-      <c r="F190" s="5"/>
+      <c r="D190" s="6"/>
+      <c r="F190" s="4"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="12"/>
       <c r="B191" s="12"/>
-      <c r="D191" s="8"/>
-      <c r="F191" s="5"/>
+      <c r="D191" s="7"/>
+      <c r="F191" s="4"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="12"/>
       <c r="B192" s="12"/>
-      <c r="D192" s="7"/>
-      <c r="F192" s="5"/>
+      <c r="D192" s="6"/>
+      <c r="F192" s="4"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="12"/>
-      <c r="D193" s="9"/>
-      <c r="F193" s="5"/>
+      <c r="D193" s="8"/>
+      <c r="F193" s="4"/>
     </row>
     <row r="194" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="12"/>
-      <c r="D194" s="7"/>
-      <c r="F194" s="5"/>
+      <c r="D194" s="6"/>
+      <c r="F194" s="4"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
       <c r="B195" s="12"/>
-      <c r="D195" s="7"/>
-      <c r="F195" s="5"/>
+      <c r="D195" s="6"/>
+      <c r="F195" s="4"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
       <c r="B196" s="12"/>
-      <c r="D196" s="7"/>
-      <c r="F196" s="5"/>
+      <c r="D196" s="6"/>
+      <c r="F196" s="4"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="12"/>
-      <c r="D197" s="8"/>
-      <c r="F197" s="5"/>
+      <c r="D197" s="7"/>
+      <c r="F197" s="4"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="12"/>
       <c r="B198" s="12"/>
-      <c r="D198" s="7"/>
-      <c r="F198" s="5"/>
+      <c r="D198" s="6"/>
+      <c r="F198" s="4"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
-      <c r="D199" s="7"/>
-      <c r="F199" s="5"/>
+      <c r="D199" s="6"/>
+      <c r="F199" s="4"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="12"/>
       <c r="B200" s="12"/>
-      <c r="D200" s="8"/>
-      <c r="F200" s="5"/>
+      <c r="D200" s="7"/>
+      <c r="F200" s="4"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="12"/>
       <c r="B201" s="12"/>
-      <c r="D201" s="9"/>
-      <c r="F201" s="5"/>
+      <c r="D201" s="8"/>
+      <c r="F201" s="4"/>
     </row>
     <row r="202" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12"/>
       <c r="B202" s="12"/>
-      <c r="D202" s="7"/>
-      <c r="F202" s="5"/>
+      <c r="D202" s="6"/>
+      <c r="F202" s="4"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="12"/>
       <c r="B203" s="12"/>
-      <c r="D203" s="8"/>
-      <c r="F203" s="5"/>
+      <c r="D203" s="7"/>
+      <c r="F203" s="4"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
       <c r="B204" s="12"/>
-      <c r="D204" s="7"/>
-      <c r="F204" s="5"/>
+      <c r="D204" s="6"/>
+      <c r="F204" s="4"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
       <c r="B205" s="12"/>
-      <c r="D205" s="9"/>
-      <c r="F205" s="5"/>
+      <c r="D205" s="8"/>
+      <c r="F205" s="4"/>
     </row>
     <row r="206" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12"/>
       <c r="B206" s="12"/>
-      <c r="D206" s="7"/>
-      <c r="F206" s="5"/>
+      <c r="D206" s="6"/>
+      <c r="F206" s="4"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="12"/>
       <c r="B207" s="12"/>
-      <c r="D207" s="7"/>
-      <c r="F207" s="5"/>
+      <c r="D207" s="6"/>
+      <c r="F207" s="4"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="12"/>
       <c r="B208" s="12"/>
-      <c r="D208" s="8"/>
-      <c r="F208" s="5"/>
+      <c r="D208" s="7"/>
+      <c r="F208" s="4"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="12"/>
       <c r="B209" s="12"/>
-      <c r="D209" s="9"/>
-      <c r="F209" s="5"/>
+      <c r="D209" s="8"/>
+      <c r="F209" s="4"/>
     </row>
     <row r="210" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="12"/>
       <c r="B210" s="12"/>
-      <c r="D210" s="7"/>
-      <c r="F210" s="5"/>
+      <c r="D210" s="6"/>
+      <c r="F210" s="4"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
       <c r="B211" s="12"/>
-      <c r="D211" s="7"/>
-      <c r="F211" s="5"/>
+      <c r="D211" s="6"/>
+      <c r="F211" s="4"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
       <c r="B212" s="12"/>
-      <c r="D212" s="8"/>
-      <c r="F212" s="5"/>
+      <c r="D212" s="7"/>
+      <c r="F212" s="4"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="12"/>
-      <c r="D213" s="9"/>
-      <c r="F213" s="5"/>
+      <c r="D213" s="8"/>
+      <c r="F213" s="4"/>
     </row>
     <row r="214" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="12"/>
-      <c r="D214" s="7"/>
-      <c r="F214" s="5"/>
+      <c r="D214" s="6"/>
+      <c r="F214" s="4"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="12"/>
       <c r="B215" s="12"/>
-      <c r="D215" s="7"/>
-      <c r="F215" s="5"/>
+      <c r="D215" s="6"/>
+      <c r="F215" s="4"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="12"/>
       <c r="B216" s="12"/>
-      <c r="D216" s="8"/>
-      <c r="F216" s="5"/>
+      <c r="D216" s="7"/>
+      <c r="F216" s="4"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="12"/>
       <c r="B217" s="12"/>
-      <c r="D217" s="9"/>
-      <c r="F217" s="5"/>
+      <c r="D217" s="8"/>
+      <c r="F217" s="4"/>
     </row>
     <row r="218" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
       <c r="B218" s="12"/>
-      <c r="D218" s="7"/>
-      <c r="F218" s="5"/>
+      <c r="D218" s="6"/>
+      <c r="F218" s="4"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="12"/>
       <c r="B219" s="12"/>
-      <c r="D219" s="7"/>
-      <c r="F219" s="5"/>
+      <c r="D219" s="6"/>
+      <c r="F219" s="4"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="12"/>
       <c r="B220" s="12"/>
-      <c r="D220" s="7"/>
-      <c r="F220" s="5"/>
+      <c r="D220" s="6"/>
+      <c r="F220" s="4"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="12"/>
       <c r="B221" s="12"/>
-      <c r="D221" s="8"/>
-      <c r="F221" s="5"/>
+      <c r="D221" s="7"/>
+      <c r="F221" s="4"/>
     </row>
     <row r="222" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="12"/>
       <c r="B222" s="12"/>
-      <c r="D222" s="7"/>
-      <c r="F222" s="5"/>
+      <c r="D222" s="6"/>
+      <c r="F222" s="4"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
       <c r="B223" s="12"/>
-      <c r="D223" s="8"/>
-      <c r="F223" s="5"/>
+      <c r="D223" s="7"/>
+      <c r="F223" s="4"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="12"/>
       <c r="B224" s="12"/>
-      <c r="D224" s="7"/>
-      <c r="F224" s="5"/>
+      <c r="D224" s="6"/>
+      <c r="F224" s="4"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="12"/>
       <c r="B225" s="12"/>
-      <c r="D225" s="9"/>
-      <c r="F225" s="5"/>
+      <c r="D225" s="8"/>
+      <c r="F225" s="4"/>
     </row>
     <row r="226" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="12"/>
       <c r="B226" s="12"/>
-      <c r="D226" s="8"/>
-      <c r="F226" s="5"/>
+      <c r="D226" s="7"/>
+      <c r="F226" s="4"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="12"/>
       <c r="B227" s="12"/>
-      <c r="D227" s="7"/>
-      <c r="F227" s="5"/>
+      <c r="D227" s="6"/>
+      <c r="F227" s="4"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
       <c r="B228" s="12"/>
-      <c r="D228" s="7"/>
-      <c r="F228" s="5"/>
+      <c r="D228" s="6"/>
+      <c r="F228" s="4"/>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="12"/>
       <c r="B229" s="12"/>
-      <c r="D229" s="9"/>
-      <c r="F229" s="4"/>
+      <c r="D229" s="8"/>
+      <c r="F229" s="3"/>
     </row>
     <row r="230" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12"/>
       <c r="B230" s="12"/>
-      <c r="D230" s="7"/>
-      <c r="F230" s="5"/>
+      <c r="D230" s="6"/>
+      <c r="F230" s="4"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="12"/>
       <c r="B231" s="12"/>
-      <c r="D231" s="7"/>
-      <c r="F231" s="5"/>
+      <c r="D231" s="6"/>
+      <c r="F231" s="4"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="12"/>
       <c r="B232" s="12"/>
-      <c r="D232" s="8"/>
-      <c r="F232" s="5"/>
+      <c r="D232" s="7"/>
+      <c r="F232" s="4"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="12"/>
       <c r="B233" s="12"/>
-      <c r="D233" s="9"/>
-      <c r="F233" s="5"/>
+      <c r="D233" s="8"/>
+      <c r="F233" s="4"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="12"/>
       <c r="B234" s="12"/>
-      <c r="D234" s="8"/>
-      <c r="F234" s="5"/>
+      <c r="D234" s="7"/>
+      <c r="F234" s="4"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="12"/>
       <c r="B235" s="12"/>
-      <c r="D235" s="7"/>
-      <c r="F235" s="5"/>
+      <c r="D235" s="6"/>
+      <c r="F235" s="4"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="12"/>
       <c r="B236" s="12"/>
-      <c r="D236" s="7"/>
-      <c r="F236" s="5"/>
+      <c r="D236" s="6"/>
+      <c r="F236" s="4"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="12"/>
       <c r="B237" s="12"/>
-      <c r="D237" s="9"/>
-      <c r="F237" s="4"/>
+      <c r="D237" s="8"/>
+      <c r="F237" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B206:B209"/>
-    <mergeCell ref="A206:A209"/>
-    <mergeCell ref="B202:B205"/>
-    <mergeCell ref="A202:A205"/>
-    <mergeCell ref="B198:B201"/>
-    <mergeCell ref="A198:A201"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B234:B237"/>
-    <mergeCell ref="A234:A237"/>
-    <mergeCell ref="B230:B233"/>
-    <mergeCell ref="A230:A233"/>
-    <mergeCell ref="B226:B229"/>
-    <mergeCell ref="A226:A229"/>
-    <mergeCell ref="B222:B225"/>
-    <mergeCell ref="A222:A225"/>
-    <mergeCell ref="B218:B221"/>
-    <mergeCell ref="A218:A221"/>
-    <mergeCell ref="B214:B217"/>
-    <mergeCell ref="A214:A217"/>
-    <mergeCell ref="B210:B213"/>
-    <mergeCell ref="A210:A213"/>
-    <mergeCell ref="B182:B185"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="B174:B177"/>
-    <mergeCell ref="A174:A177"/>
-    <mergeCell ref="B194:B197"/>
-    <mergeCell ref="A194:A197"/>
-    <mergeCell ref="B190:B193"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="B186:B189"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B158:B161"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="A150:A153"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="B162:B165"/>
-    <mergeCell ref="A162:A165"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B130:B133"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="B126:B129"/>
-    <mergeCell ref="A126:A129"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="A146:A149"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="A142:A145"/>
-    <mergeCell ref="B138:B141"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="A110:A113"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="A102:A105"/>
-    <mergeCell ref="B122:B125"/>
-    <mergeCell ref="A122:A125"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="A118:A121"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="A114:A117"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="A38:A41"/>
@@ -2130,11 +2113,104 @@
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="A122:A125"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="B126:B129"/>
+    <mergeCell ref="A126:A129"/>
+    <mergeCell ref="B146:B149"/>
+    <mergeCell ref="A146:A149"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="A142:A145"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="B214:B217"/>
+    <mergeCell ref="A214:A217"/>
+    <mergeCell ref="B210:B213"/>
+    <mergeCell ref="A210:A213"/>
+    <mergeCell ref="B182:B185"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="B174:B177"/>
+    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="B194:B197"/>
+    <mergeCell ref="A194:A197"/>
+    <mergeCell ref="B190:B193"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="B186:B189"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B234:B237"/>
+    <mergeCell ref="A234:A237"/>
+    <mergeCell ref="B230:B233"/>
+    <mergeCell ref="A230:A233"/>
+    <mergeCell ref="B226:B229"/>
+    <mergeCell ref="A226:A229"/>
+    <mergeCell ref="B222:B225"/>
+    <mergeCell ref="A222:A225"/>
+    <mergeCell ref="B218:B221"/>
+    <mergeCell ref="A218:A221"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B206:B209"/>
+    <mergeCell ref="A206:A209"/>
+    <mergeCell ref="B202:B205"/>
+    <mergeCell ref="A202:A205"/>
+    <mergeCell ref="B198:B201"/>
+    <mergeCell ref="A198:A201"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B158:B161"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="A150:A153"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B130:B133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2161,183 +2237,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="13"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="13"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="13"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A6:A9"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A18:A21"/>
@@ -2350,14 +2434,6 @@
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2382,19 +2458,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>